<commit_message>
Update .gitignore to include harvest_summary.xlsx and modify plant index PDFs
</commit_message>
<xml_diff>
--- a/df/harvest_summary.xlsx
+++ b/df/harvest_summary.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,7 +519,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>75.31999999999999</v>
+        <v>80.62</v>
       </c>
       <c r="F2" s="3" t="inlineStr"/>
       <c r="G2" s="4">
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>40.02</v>
+        <v>47.52</v>
       </c>
       <c r="F3" s="3" t="inlineStr"/>
       <c r="G3" s="4">
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>30.61</v>
+        <v>33.61</v>
       </c>
       <c r="F5" s="3" t="inlineStr"/>
       <c r="G5" s="4">
@@ -631,7 +631,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="3" t="inlineStr"/>
       <c r="G6" s="4">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.99</v>
+        <v>3.19</v>
       </c>
       <c r="F8" s="3" t="inlineStr"/>
       <c r="G8" s="4">
@@ -697,25 +697,25 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Onion</t>
+          <t>Swiss Chard</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Yellow store bought propogation</t>
+          <t>Ruby Red</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Ounces</t>
+          <t>Bunches</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3.2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="3" t="inlineStr"/>
       <c r="G9" s="4">
@@ -725,25 +725,25 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Garlic</t>
+          <t>Onion</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yellow store bought propogation</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Each</t>
+          <t>Ounces</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>3.2</v>
       </c>
       <c r="F10" s="3" t="inlineStr"/>
       <c r="G10" s="4">
@@ -751,15 +751,43 @@
         <v/>
       </c>
     </row>
-    <row r="11"/>
-    <row r="12">
-      <c r="F12" t="inlineStr">
+    <row r="11">
+      <c r="A11" t="n">
+        <v>28</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Garlic</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Each</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="inlineStr"/>
+      <c r="G11" s="4">
+        <f>E11*F11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12"/>
+    <row r="13">
+      <c r="F13" t="inlineStr">
         <is>
           <t>Total Harvest Value:</t>
         </is>
       </c>
-      <c r="G12" s="5">
-        <f>SUM(G2:G11)</f>
+      <c r="G13" s="5">
+        <f>SUM(G2:G12)</f>
         <v/>
       </c>
     </row>

</xml_diff>